<commit_message>
didn't really do anything
</commit_message>
<xml_diff>
--- a/new_brm.xlsx
+++ b/new_brm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livemissouristate-my.sharepoint.com/personal/eri2005_missouristate_edu/Documents/RESEARCH/2 projects/Table-of-Doom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Missouri State University/RESEARCH/2 projects/Table-of-Doom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140008_{F64CFD53-C1F0-EE48-9548-EF0DCEDE7D6E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6A639B64-3E3D-4D46-9CCC-D9C7E6E0B08E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1260" windowWidth="25600" windowHeight="13940"/>
+    <workbookView xWindow="0" yWindow="1260" windowWidth="25600" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new_brm" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="391">
   <si>
     <t>Item Title</t>
   </si>
@@ -1190,13 +1190,19 @@
   </si>
   <si>
     <t>Angela Nogueira N. B. CampanaMaria da Consola√ß√£o Gomes Cunha Fernandes TavaresDirceu da SilvaMaria Jose D'Elboux Diogo</t>
+  </si>
+  <si>
+    <t>MultiPic: A standardized set of 750 drawings with norms for six European languages</t>
+  </si>
+  <si>
+    <t>Not BRM but need</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1311,6 +1317,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="TimesNewRomanPSMT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="TimesNewRomanPSMT"/>
       <family val="2"/>
     </font>
@@ -1612,7 +1625,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1655,11 +1668,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1693,6 +1708,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2033,11 +2049,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J95"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
-      <selection activeCell="I95" sqref="I95"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4680,14 +4696,25 @@
         <v>11</v>
       </c>
     </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B96" t="s">
+        <v>390</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:J311">
     <sortCondition ref="A1"/>
   </sortState>
-  <conditionalFormatting sqref="A12:A1048576 A1:A10">
+  <conditionalFormatting sqref="A12:A95 A1:A10 A97:A1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A96" r:id="rId1" display="javascript:void(0)" xr:uid="{FDFFE69C-8105-6245-B4B3-0D85CE3EE2C4}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>